<commit_message>
added streamlit ui with chat bot
</commit_message>
<xml_diff>
--- a/python-streamlit/bereavement_train.xlsx
+++ b/python-streamlit/bereavement_train.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vinayak\fullstack\bereavement\bereavement\python-streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59B24F4-AEE1-489A-A1BC-F3BEA5ADA6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7589A8A2-8D81-411C-899A-60B437BC820C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B4B9AE63-311E-483B-A6DB-237C1B8C8E6F}"/>
   </bookViews>
@@ -708,7 +708,7 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>